<commit_message>
Fix UpToDate link format issue
</commit_message>
<xml_diff>
--- a/check_links/checked_links.xlsx
+++ b/check_links/checked_links.xlsx
@@ -2818,20 +2818,20 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Valacyclovir</t>
+          <t>valacyclovir</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>https://www.uptodate.com/contents/Valacyclovir-drug-information</t>
+          <t>https://www.uptodate.com/contents/valacyclovir-drug-information</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://www.uptodate.com/contents/valacyclovir-drug-information</t>
         </is>
       </c>
     </row>
@@ -19652,11 +19652,11 @@
         </is>
       </c>
       <c r="D769" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="E769" t="inlineStr">
         <is>
-          <t>https://www.uptodate.com/contents/sodium-chloride-preparations-saline-and-oral-salt-tablets-drug-information</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>